<commit_message>
Survey Station at Sea Creation
Created a "survey station at sea" Rmd file.  Enter the next stations you'd like to do in the order of your choosing, then output the cumulative station table with grid ID and a map showing the station locations
</commit_message>
<xml_diff>
--- a/Data/WGOA station_list_dougherty_2019_ProjInstrutions.xlsx
+++ b/Data/WGOA station_list_dougherty_2019_ProjInstrutions.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">All!$A$1:$E$273</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1245,7 +1248,7 @@
   <dimension ref="A1:E273"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E117" sqref="E117:E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>